<commit_message>
Updated concordance table with test line
</commit_message>
<xml_diff>
--- a/data/Konkordanztabellen/konkordanz_historia-francorum.xlsx
+++ b/data/Konkordanztabellen/konkordanz_historia-francorum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pschneider/Documents/DH-Projekte/Digital Methods in Practice/data/Konkordanztabellen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85143C06-6FE5-0448-B4B0-4ECFBC834907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F2B469-015A-3049-8CFD-079276E7ACE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="28040" windowHeight="17100" xr2:uid="{313A6262-6311-C14B-93F5-B76954400F72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>historia-francorum_zeile</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Ps</t>
+  </si>
+  <si>
+    <t>dies ist ein längeres Zitat, das so auch im anderen Text auftaucht und von Tracer gefunden werden müsste tertius.</t>
+  </si>
+  <si>
+    <t>ad dies ist ein längeres Zitat, das so auch im anderen Text auftaucht und von Tracer gefunden werden müsste.</t>
   </si>
 </sst>
 </file>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31D425-11AF-3A48-B021-59875D9E01F1}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,135 +548,129 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1200000227</v>
+        <v>1200000008</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D2">
-        <v>1100014246</v>
+        <v>1100000013</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1200000258</v>
+        <v>1200000227</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>1100014598</v>
+        <v>1100014246</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1200000260</v>
+        <v>1200000258</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>1100014031</v>
+        <v>1100014598</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1200000396</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>1200000260</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>1100014089</v>
+        <v>1100014031</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1200000406</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
+        <v>1200000396</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6">
-        <v>1100014250</v>
+        <v>1100014089</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1200000438</v>
+        <v>1200000406</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <v>1100014250</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1200000484</v>
+        <v>1200000438</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8">
-        <v>1100014379</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1200000485</v>
+        <v>1200000484</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -681,77 +681,97 @@
       <c r="E9" t="s">
         <v>30</v>
       </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1200000798</v>
+        <v>1200000485</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
       </c>
       <c r="D10">
-        <v>1100028674</v>
+        <v>1100014379</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1200000864</v>
+        <v>1200000798</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11">
-        <v>1100024121</v>
+        <v>1100028674</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1200001125</v>
+        <v>1200000864</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D12">
-        <v>1100015733</v>
+        <v>1100024121</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1200001250</v>
+        <v>1200001125</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13">
-        <v>1100015893</v>
+        <v>1100015733</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>1200001250</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>1100015893</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>1200001290</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>